<commit_message>
update: return validate file import teacher
</commit_message>
<xml_diff>
--- a/public/files/teacher_template.xlsx
+++ b/public/files/teacher_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HTTT\DoAnTN\Project\FE3\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B05077-FD32-4569-97A7-CE60E8F7E5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1470ECD-03AB-47D0-8691-C5E737336DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B8962491-F3BD-455F-A1CF-BA3E487930C5}"/>
   </bookViews>
@@ -66,6 +66,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,9 +104,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +446,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,7 +454,7 @@
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="5" width="19.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="3" customWidth="1"/>
     <col min="7" max="7" width="19.77734375" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
@@ -470,7 +475,7 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">

</xml_diff>